<commit_message>
Seriennummer, Name, Korrekte HW-Nummer
</commit_message>
<xml_diff>
--- a/ProductionTests/Stuv2.1.4.xlsx
+++ b/ProductionTests/Stuv2.1.4.xlsx
@@ -2,22 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16896" windowWidth="30936" xWindow="15252" yWindow="-108"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Product Data@0x4" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Statistics@0x5" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,20 +27,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b val="1"/>
       <sz val="20"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,14 +54,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Standard" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -366,23 +357,23 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="43.140625"/>
-    <col customWidth="1" max="2" min="2" width="14.42578125"/>
-    <col customWidth="1" max="3" min="3" width="12.85546875"/>
-    <col customWidth="1" max="4" min="4" width="17.5703125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="255.7109375"/>
-    <col customWidth="1" max="6" min="6" width="9.5703125"/>
-    <col customWidth="1" max="7" min="7" width="12.85546875"/>
-    <col customWidth="1" max="8" min="8" width="104.42578125"/>
+    <col customWidth="1" max="1" min="1" width="43.2"/>
+    <col customWidth="1" max="2" min="2" width="14.4"/>
+    <col customWidth="1" max="3" min="3" width="12.8"/>
+    <col customWidth="1" max="4" min="4" width="17.6"/>
+    <col customWidth="1" max="5" min="5" width="84"/>
+    <col customWidth="1" max="6" min="6" width="9.600000000000001"/>
+    <col customWidth="1" max="7" min="7" width="12.8"/>
+    <col customWidth="1" max="8" min="8" width="144"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26.25" r="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
@@ -424,7 +415,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2">
+    <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>GTIN</t>
@@ -441,10 +432,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="inlineStr">
@@ -458,7 +447,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="3">
+    <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Hardware Revision - Reserved</t>
@@ -475,10 +464,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="n"/>
       <c r="G3" s="2" t="inlineStr">
@@ -492,7 +479,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="4">
+    <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Hardware Revision - Major</t>
@@ -509,10 +496,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E4" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="n"/>
       <c r="G4" s="2" t="inlineStr">
@@ -526,7 +511,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="5">
+    <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Hardware Revision - Minor</t>
@@ -543,10 +528,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E5" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="inlineStr">
@@ -560,10 +543,10 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="6">
+    <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Hardware Revision - Build</t>
+          <t>Hardware Revision - Revision</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -577,10 +560,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="n"/>
       <c r="G6" s="2" t="inlineStr">
@@ -594,7 +575,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="7">
+    <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Firmware Version Number - Reserved</t>
@@ -611,10 +592,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F7" s="2" t="n"/>
       <c r="G7" s="2" t="inlineStr">
@@ -628,7 +607,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="8">
+    <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Firmware Version Number - Major</t>
@@ -645,10 +624,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E8" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="F8" s="2" t="n"/>
       <c r="G8" s="2" t="inlineStr">
@@ -662,7 +639,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="9">
+    <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Firmware Version Number - Minor</t>
@@ -679,10 +656,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E9" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F9" s="2" t="n"/>
       <c r="G9" s="2" t="inlineStr">
@@ -696,7 +671,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="10">
+    <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Firmware Version Number - Build</t>
@@ -713,10 +688,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="E10" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="F10" s="2" t="n"/>
       <c r="G10" s="2" t="inlineStr">
@@ -730,7 +703,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="11">
+    <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Release Name</t>
@@ -749,7 +722,7 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>Tanja</t>
+          <t>Valerie</t>
         </is>
       </c>
       <c r="F11" s="2" t="n"/>
@@ -764,7 +737,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="12">
+    <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Serial Number</t>
@@ -783,7 +756,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>MyToolItStu001-1-00001-001-2</t>
         </is>
       </c>
       <c r="F12" s="2" t="n"/>
@@ -794,11 +767,11 @@
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>Manufactor Serial Number</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="13">
+          <t>Manufactor Serial Number (Derived from ISBN); Product Group - Subgroup - Manufacture ID - Product Number - Check Digit</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Name</t>
@@ -817,7 +790,7 @@
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Digital and Analog Communication with 5V-Supply - www.ico-tronic.com</t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -832,7 +805,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="14">
+    <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
           <t>OEM Free Use</t>
@@ -849,10 +822,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>[0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0, 0x0]</t>
-        </is>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F14" s="2" t="n"/>
       <c r="G14" s="2" t="n"/>
@@ -876,22 +847,22 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H8"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="52.85546875"/>
-    <col customWidth="1" max="2" min="2" width="14.42578125"/>
-    <col customWidth="1" max="3" min="3" width="12.85546875"/>
-    <col customWidth="1" max="4" min="4" width="17.5703125"/>
-    <col customWidth="1" max="5" min="5" width="11.140625"/>
-    <col customWidth="1" max="6" min="6" width="10.85546875"/>
-    <col customWidth="1" max="7" min="7" width="12.85546875"/>
-    <col customWidth="1" max="8" min="8" width="99.5703125"/>
+    <col customWidth="1" max="1" min="1" width="52.8"/>
+    <col customWidth="1" max="2" min="2" width="14.4"/>
+    <col customWidth="1" max="3" min="3" width="12.8"/>
+    <col customWidth="1" max="4" min="4" width="17.6"/>
+    <col customWidth="1" max="5" min="5" width="11.2"/>
+    <col customWidth="1" max="6" min="6" width="10.8"/>
+    <col customWidth="1" max="7" min="7" width="12.8"/>
+    <col customWidth="1" max="8" min="8" width="99.59999999999999"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26.25" r="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
@@ -933,7 +904,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2">
+    <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Power On Cylces</t>
@@ -950,10 +921,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="inlineStr">
@@ -967,7 +936,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="3">
+    <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Power Off Cylces</t>
@@ -984,10 +953,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="n"/>
       <c r="G3" s="2" t="inlineStr">
@@ -1001,7 +968,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="4">
+    <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Operating Time since first power On</t>
@@ -1018,10 +985,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
@@ -1039,7 +1004,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="5">
+    <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Under Voltage Counter since first Power On</t>
@@ -1056,10 +1021,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="inlineStr">
@@ -1073,7 +1036,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="6">
+    <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Watchdog Reset Counter </t>
@@ -1090,10 +1053,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="n"/>
       <c r="G6" s="2" t="inlineStr">
@@ -1107,7 +1068,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="7">
+    <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Production Date</t>
@@ -1124,10 +1085,8 @@
           <t>True</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>20191009</t>
-        </is>
+      <c r="E7" s="2" t="n">
+        <v>20190910</v>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
@@ -1145,35 +1104,33 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="8">
-      <c r="A8" s="3" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Batch Number</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>unsigned</t>
-        </is>
-      </c>
-      <c r="H8" s="3" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>unsigned</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
         <is>
           <t>Consecutive number for manufactured devices</t>
         </is>
@@ -1181,6 +1138,5 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>